<commit_message>
Provide medical professionals with fillable and printable medical forms
Adds a "Medical Forms" tab to OutpatientConsultation.tsx with Clinical Summary, Medical Report, Referral Out, and Lab Request forms.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e19ec2c4-9b88-476b-a796-f78a3d8889e5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/87d38bc8-8976-4395-86ac-1539bdc467fb/e8597837-82ec-4b67-ac5c-6c402e7dc326.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/MEDICAL REPORT OFFICIAL.xlsx
+++ b/attached_assets/MEDICAL REPORT OFFICIAL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\OD-PC1\Public\LAB TEMPLATES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\OD-PC1\docs\INVOICES 2025\MAKL 2025\ERICK MWANGI WACHIRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>MEDICAL REPORT</t>
   </si>
@@ -79,6 +79,90 @@
   </si>
   <si>
     <t>DF</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>P.O Diazepam 10mg TDS x 3/7, 10mg BD x 3/7, 10mg OD x 3/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychotherapy - Individual, Group    </t>
+  </si>
+  <si>
+    <t>LAB TO BE DONE:</t>
+  </si>
+  <si>
+    <t>15b/min</t>
+  </si>
+  <si>
+    <t>37.4 degrees celsius</t>
+  </si>
+  <si>
+    <t>Due to the above complaints, the patient has been recommended to undergo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He was accesed using the CAGE and MMSE in which he scored high and was thus recommended to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">undergo pharmachotherapy and pscyhotherapy for better results. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weak, and has tremors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the 90 days rehabilitation program for full recovery. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The above patient was brought to our facility as a referal from Chiromo Lane Medical  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre with complaints of chronic alcohol use, tremens delirium, confusion and random anger outburts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBS                                   VDRL                        mRDT                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        HIV                           Urinalysis                 Urine toxicology </t>
+  </si>
+  <si>
+    <t>148/75mmHG</t>
+  </si>
+  <si>
+    <t>88b/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O Mirtazapine Nocte x 2/52        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P.O Carbamazepine 200mg BD x 2/52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On admission, he is sick looking, severely intoxicated. </t>
+  </si>
+  <si>
+    <t>ERICK WACHIRA</t>
+  </si>
+  <si>
+    <t>40 YEARS</t>
+  </si>
+  <si>
+    <t>25/02/2025</t>
+  </si>
+  <si>
+    <t>HESBON OBURE</t>
+  </si>
+  <si>
+    <t>The patient is faily kempt,  his speech is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> partially oriented to time, place and person, Behaviour- withdrawn, judgement- partial</t>
+  </si>
+  <si>
+    <t>decreased in rate, rhythm and  volume, mood - low, affect - incongruent, partial insight,</t>
+  </si>
+  <si>
+    <t>Alcohol Abuse with intoxication/ Major Depressive Disorder/ Diabetes Mellitus</t>
   </si>
 </sst>
 </file>
@@ -209,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -277,6 +361,34 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -284,20 +396,8 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -656,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K54"/>
+  <dimension ref="A2:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -693,23 +793,29 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="16"/>
+      <c r="H5" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="J5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" s="17" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -718,14 +824,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
+      <c r="D7" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" s="17" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -733,18 +841,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
+      <c r="C9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="24"/>
+      <c r="A10" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -757,169 +869,185 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
+      <c r="A11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A12" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-    </row>
-    <row r="16" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="F14" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="10" t="s">
+      <c r="B18" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="11" t="s">
+      <c r="E18" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="3" t="s">
+      <c r="H18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="J18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-    </row>
-    <row r="22" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-    </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-    </row>
-    <row r="26" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A22" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A24" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-    </row>
-    <row r="28" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-    </row>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+    </row>
+    <row r="27" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="30" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A31" s="24"/>
+      <c r="A31" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
@@ -932,61 +1060,69 @@
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
     </row>
     <row r="34" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A35" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
     </row>
     <row r="36" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A39" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A41" s="24"/>
+      <c r="A41" s="24" t="s">
+        <v>21</v>
+      </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
       <c r="D41" s="24"/>
@@ -1000,7 +1136,9 @@
     </row>
     <row r="42" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A43" s="24"/>
+      <c r="A43" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
@@ -1013,119 +1151,110 @@
       <c r="K43" s="24"/>
     </row>
     <row r="44" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
     </row>
     <row r="46" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A47" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
     </row>
     <row r="48" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="24"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
     </row>
     <row r="50" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
+    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H53" s="18"/>
-      <c r="I53" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-    </row>
-    <row r="54" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="D39:K39"/>
+  <mergeCells count="27">
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="A39:K39"/>
     <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A37:K37"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A45:K45"/>
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="C9:K9"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="A22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.83333333333333337" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader xml:space="preserve">&amp;C&amp;"Tahoma,Bold"&amp;20&amp;K8E1C10LIFEBRIDGE C. HOSPITAL&amp;"Tahoma,Regular"&amp;8&amp;K03+000
 &amp;"Tahoma,Bold"&amp;11COMPREHENSIVE MENTAL HEALTH&amp;R&amp;"Tahoma,Bold"&amp;K03+0000725133444 | 0732313173
@@ -1133,7 +1262,7 @@
 www.lifebridgehospital.org </oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="54" max="16383" man="1"/>
+    <brk id="52" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Enable generating printable forms with branding for clinical documentation
Adds ClinicalSummaryForm, DischargeSummaryForm, and TreatmentRecordForm components with print/download functionality.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e19ec2c4-9b88-476b-a796-f78a3d8889e5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/87d38bc8-8976-4395-86ac-1539bdc467fb/0caa38e2-0415-42c4-9166-5249d7a59c2c.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/MEDICAL REPORT OFFICIAL.xlsx
+++ b/attached_assets/MEDICAL REPORT OFFICIAL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\OD-PC1\docs\INVOICES 2025\MAKL 2025\ERICK MWANGI WACHIRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\OD-PC1\docs\INVOICES 2025\MAKL 2025\MICHAEL MBUGUA NJUGUNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>MEDICAL REPORT</t>
   </si>
@@ -81,95 +81,101 @@
     <t>DF</t>
   </si>
   <si>
+    <t>P.O Diazepam 10mg TDS x 3/7, 10mg BD x 3/7, 10mg OD x 3/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBS                                   VDRL                        mRDT                     CRP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D - dimer                            UECS                        LFTS                       TFT  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychotherapy - Individual, Group    </t>
+  </si>
+  <si>
+    <t>IV Pabrinex I and II in 500mls of D5 OD for 5 days      P.O Carbamazepine 200mg BD x 2/52</t>
+  </si>
+  <si>
+    <t>has delusions,  hallucinations, is not oriented to time, place and person</t>
+  </si>
+  <si>
+    <t>LAB TO BE DONE:</t>
+  </si>
+  <si>
+    <t>36.4 degrees celsius</t>
+  </si>
+  <si>
+    <t>88b/min</t>
+  </si>
+  <si>
+    <t>14b/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O Naltrexone BD x 2/52        </t>
+  </si>
+  <si>
+    <t>chronic use of alcohol, tremors, confusion , talking a lot, visual and auditory hallucinations, random flashbacks</t>
+  </si>
+  <si>
+    <t>increased in rate, rhythm and high in  volume, mood - low, affect - incongruent, has no insight,</t>
+  </si>
+  <si>
+    <t>Due to the above complaints, the patient has been recommended to undergo</t>
+  </si>
+  <si>
+    <t>intensive pharmachotherapy and psychotherapy for better results.</t>
+  </si>
+  <si>
+    <t>lack of sleep and restlessness. No rapport was established due to the patient being severely intoxicated and</t>
+  </si>
+  <si>
+    <t>management under close monitoring</t>
+  </si>
+  <si>
     <t>MALE</t>
   </si>
   <si>
-    <t>P.O Diazepam 10mg TDS x 3/7, 10mg BD x 3/7, 10mg OD x 3/7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psychotherapy - Individual, Group    </t>
-  </si>
-  <si>
-    <t>LAB TO BE DONE:</t>
-  </si>
-  <si>
-    <t>15b/min</t>
-  </si>
-  <si>
-    <t>37.4 degrees celsius</t>
-  </si>
-  <si>
-    <t>Due to the above complaints, the patient has been recommended to undergo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He was accesed using the CAGE and MMSE in which he scored high and was thus recommended to </t>
-  </si>
-  <si>
-    <t xml:space="preserve">undergo pharmachotherapy and pscyhotherapy for better results. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">weak, and has tremors. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">the 90 days rehabilitation program for full recovery. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The above patient was brought to our facility as a referal from Chiromo Lane Medical  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre with complaints of chronic alcohol use, tremens delirium, confusion and random anger outburts. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RBS                                   VDRL                        mRDT                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        HIV                           Urinalysis                 Urine toxicology </t>
-  </si>
-  <si>
-    <t>148/75mmHG</t>
-  </si>
-  <si>
-    <t>88b/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.O Mirtazapine Nocte x 2/52        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P.O Carbamazepine 200mg BD x 2/52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On admission, he is sick looking, severely intoxicated. </t>
-  </si>
-  <si>
-    <t>ERICK WACHIRA</t>
-  </si>
-  <si>
-    <t>40 YEARS</t>
-  </si>
-  <si>
-    <t>25/02/2025</t>
+    <t>Patient brought to our facility as a referal from Bliss Medical Centre with complaints of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disoriented to time place and person. He has thus been recommended to undergo intensive psychiatric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On admission, he is sick looking, clinically afebrile, slightly pale, </t>
+  </si>
+  <si>
+    <t>The patient is unkempt,  his speech is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHG         HIV                           Urinalysis                 Urine toxicology      </t>
   </si>
   <si>
     <t>HESBON OBURE</t>
   </si>
   <si>
-    <t>The patient is faily kempt,  his speech is</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> partially oriented to time, place and person, Behaviour- withdrawn, judgement- partial</t>
-  </si>
-  <si>
-    <t>decreased in rate, rhythm and  volume, mood - low, affect - incongruent, partial insight,</t>
-  </si>
-  <si>
-    <t>Alcohol Abuse with intoxication/ Major Depressive Disorder/ Diabetes Mellitus</t>
+    <t>178/74mmHG</t>
+  </si>
+  <si>
+    <t>MICHAEL MBUGUA NJUGUNA</t>
+  </si>
+  <si>
+    <t>31YEARS</t>
+  </si>
+  <si>
+    <t>30/05/2025</t>
+  </si>
+  <si>
+    <t>severely intoxicated, minor wounds and bruises.</t>
+  </si>
+  <si>
+    <t>Bipolar Mood Disorder/Alcohol induced psychosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color rgb="FFFFFFFF"/>
@@ -221,6 +227,11 @@
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -293,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -365,26 +376,18 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -402,6 +405,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -756,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K52"/>
+  <dimension ref="A2:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:K39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -793,29 +800,29 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="30"/>
+      <c r="J5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" s="17" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,16 +831,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="D7" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" s="17" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -841,352 +848,366 @@
         <v>5</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="24" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A11" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A12" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A23" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-    </row>
-    <row r="13" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-    </row>
-    <row r="15" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="25" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+    </row>
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A25" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="25"/>
-    </row>
-    <row r="19" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-    </row>
-    <row r="21" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A22" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-    </row>
-    <row r="23" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A24" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-    </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-    </row>
-    <row r="27" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A28" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-    </row>
-    <row r="29" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+    </row>
+    <row r="28" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A29" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+    </row>
     <row r="30" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A31" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
+      <c r="A31" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A33" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-    </row>
-    <row r="34" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A35" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A37" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+    </row>
+    <row r="38" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-    </row>
-    <row r="38" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A39" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
+      <c r="D39" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
     </row>
     <row r="40" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A41" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
+      <c r="A41" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
     </row>
     <row r="42" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A43" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
+      <c r="A43" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
     </row>
     <row r="44" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A45" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-    </row>
-    <row r="46" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A47" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
+      <c r="D47" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
     </row>
     <row r="48" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A49" s="22"/>
+      <c r="A49" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
@@ -1199,39 +1220,56 @@
       <c r="K49" s="22"/>
     </row>
     <row r="50" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
-    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+    </row>
+    <row r="52" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+    <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="32" t="s">
+      <c r="B53" s="6"/>
+      <c r="C53" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="20" t="s">
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="18"/>
-      <c r="I51" s="21" t="s">
+      <c r="H53" s="18"/>
+      <c r="I53" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="K51" s="32"/>
-    </row>
-    <row r="52" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
+      <c r="J53" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="K53" s="30"/>
+    </row>
+    <row r="54" spans="1:11" s="17" customFormat="1" ht="6.75" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="C51:F51"/>
+  <mergeCells count="32">
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="A41:K41"/>
     <mergeCell ref="A43:K43"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A41:K41"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A5:B5"/>
@@ -1239,19 +1277,21 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="C9:K9"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A31:K31"/>
     <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="A23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.83333333333333337" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1262,7 +1302,7 @@
 www.lifebridgehospital.org </oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="52" max="16383" man="1"/>
+    <brk id="54" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>